<commit_message>
se arregla el modulo length
</commit_message>
<xml_diff>
--- a/documentacion/Copy of AREA Y PERIMETER TAKEOFF (003).xlsx
+++ b/documentacion/Copy of AREA Y PERIMETER TAKEOFF (003).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rauls\OneDrive\Documentos\Pcloud2022\me3co\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\Documents\proyectos\xeon-it\me3co\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A734B73B-4FD3-4415-AFBF-9AC2423FDB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1BACF-0A07-49C5-B274-1A5C678314F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15FF0A33-CE28-4CBA-933C-B148DBA9EDB0}"/>
+    <workbookView xWindow="-28920" yWindow="-9975" windowWidth="29040" windowHeight="15720" xr2:uid="{15FF0A33-CE28-4CBA-933C-B148DBA9EDB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
   <si>
     <t>Takeoff name</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Select Materials</t>
   </si>
   <si>
-    <t>wall ties</t>
-  </si>
-  <si>
     <t>Rebar</t>
   </si>
   <si>
@@ -397,6 +394,21 @@
   </si>
   <si>
     <t>este no va, es igual que el de arriba</t>
+  </si>
+  <si>
+    <t>rebar</t>
+  </si>
+  <si>
+    <t>h9</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>i9</t>
+  </si>
+  <si>
+    <t>i4</t>
   </si>
 </sst>
 </file>
@@ -406,7 +418,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -679,15 +691,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -710,7 +718,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -740,10 +747,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,54 +1068,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EAE8C18-F56B-4B80-B8F7-533F8F5D500D}">
   <dimension ref="A2:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H106" sqref="H106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.796875" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="12.296875" customWidth="1"/>
-    <col min="5" max="5" width="16.59765625" customWidth="1"/>
-    <col min="6" max="6" width="11.69921875" customWidth="1"/>
-    <col min="7" max="7" width="24.59765625" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12.796875" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="23"/>
       <c r="C2" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3">
         <v>12</v>
@@ -1136,12 +1139,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="18">
@@ -1166,12 +1169,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="20">
         <v>12</v>
@@ -1195,12 +1198,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6">
         <v>1E-3</v>
@@ -1224,12 +1227,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="19">
         <v>0.25</v>
@@ -1253,12 +1256,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="18">
@@ -1283,12 +1286,12 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="E9" s="18">
         <v>1</v>
@@ -1312,12 +1315,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="E10" s="18">
         <v>1</v>
@@ -1341,12 +1344,12 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" s="18">
         <v>1</v>
@@ -1367,7 +1370,7 @@
       </c>
       <c r="J11" s="19"/>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="E12" s="18"/>
@@ -1377,30 +1380,30 @@
       <c r="I12" s="21"/>
       <c r="J12" s="19"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>51</v>
-      </c>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
-        <v>52</v>
       </c>
       <c r="D14">
         <v>165</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="60">
         <v>0.375</v>
       </c>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15">
         <v>200</v>
@@ -1408,9 +1411,9 @@
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>300</v>
@@ -1418,53 +1421,53 @@
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E17">
         <v>100</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18">
         <v>65.5</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E19">
         <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20">
         <v>65.5</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21">
         <f>E19*E20</f>
@@ -1474,20 +1477,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <f>E17+E18+E19+E20</f>
         <v>331</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="49" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="3"/>
@@ -1498,20 +1501,20 @@
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="78" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="73" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="77" t="s">
-        <v>56</v>
+      <c r="E25" s="72" t="s">
+        <v>55</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="78" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="73" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="1"/>
@@ -1522,20 +1525,20 @@
       <c r="F26" s="1"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="78" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
+        <v>78</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="32" t="s">
         <v>6</v>
       </c>
@@ -1548,11 +1551,11 @@
       <c r="F28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
+      <c r="G28" s="39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>5</v>
       </c>
@@ -1562,11 +1565,11 @@
         <v>0.5</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
+      <c r="G29" s="39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -1580,10 +1583,10 @@
         <v>19</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
@@ -1598,185 +1601,185 @@
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="44" t="s">
+      <c r="G33" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H33" t="s">
         <v>103</v>
       </c>
-      <c r="H33" t="s">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42">
+        <v>2</v>
+      </c>
+      <c r="F34" s="43" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46">
-        <v>2</v>
-      </c>
-      <c r="F34" s="47" t="s">
-        <v>105</v>
-      </c>
       <c r="G34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38">
         <f>E34*E22</f>
         <v>662</v>
       </c>
-      <c r="F35" s="49"/>
+      <c r="F35" s="45"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="2:10">
-      <c r="B36" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38">
         <v>0.5</v>
       </c>
-      <c r="F36" s="49"/>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42">
+      <c r="F36" s="45"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38">
         <f>SUM(E35*E36)</f>
         <v>331</v>
       </c>
-      <c r="F37" s="49" t="s">
+      <c r="F37" s="45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="46" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="2:10">
-      <c r="B38" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51">
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47">
         <f>SUM(E37/I3)</f>
         <v>12.25925925925926</v>
       </c>
-      <c r="F38" s="52"/>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="B39" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55">
+      <c r="F38" s="48"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51">
         <v>2</v>
       </c>
-      <c r="F39" s="56"/>
+      <c r="F39" s="52"/>
       <c r="G39" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="B40" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54">
         <f>SUM(E22*E39)</f>
         <v>662</v>
       </c>
-      <c r="F40" s="59"/>
-    </row>
-    <row r="41" spans="2:10">
-      <c r="B41" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58">
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54">
         <v>0.5</v>
       </c>
-      <c r="F41" s="59"/>
-    </row>
-    <row r="42" spans="2:10">
-      <c r="B42" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58">
+      <c r="F41" s="55"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54">
         <f>SUM(E40*E41)</f>
         <v>331</v>
       </c>
-      <c r="F42" s="59" t="s">
+      <c r="F42" s="55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="56" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="2:10">
-      <c r="B43" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61">
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57">
         <f>SUM(E42/I3)</f>
         <v>12.25925925925926</v>
       </c>
-      <c r="F43" s="62" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10">
+      <c r="F43" s="58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="2:10">
-      <c r="B45" s="63" t="s">
-        <v>119</v>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="59" t="s">
+        <v>118</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="10"/>
       <c r="E45" s="11"/>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10">
+      <c r="F46" s="40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>21</v>
       </c>
@@ -1785,7 +1788,7 @@
         <v>6550</v>
       </c>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="12" t="s">
         <v>11</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="49" spans="2:10">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>12</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>4323</v>
       </c>
     </row>
-    <row r="50" spans="2:10">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" s="7" t="s">
         <v>13</v>
       </c>
@@ -1813,72 +1816,72 @@
         <v>160.11111111111111</v>
       </c>
       <c r="F50" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10">
-      <c r="B51" s="45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="2:10">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="2:10">
-      <c r="B53" s="63" t="s">
-        <v>71</v>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="59" t="s">
+        <v>70</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="10"/>
       <c r="E53" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" t="s">
         <v>114</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G53" s="64" t="s">
+      <c r="H53" t="s">
         <v>115</v>
       </c>
-      <c r="H53" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="I53" s="64" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10">
+      <c r="I53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F54" s="6">
         <f>E21</f>
         <v>6550</v>
       </c>
     </row>
-    <row r="55" spans="2:10">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="E55">
-        <v>0.56200000000000006</v>
+        <v>1.5</v>
       </c>
       <c r="F55" s="6">
         <f>SUM(F54*E55)</f>
-        <v>3681.1000000000004</v>
+        <v>9825</v>
       </c>
       <c r="G55" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E56">
         <v>2.5</v>
@@ -1888,7 +1891,7 @@
         <v>16375</v>
       </c>
       <c r="G56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H56">
         <f>F56/H4</f>
@@ -1903,9 +1906,9 @@
         <v>3.0703125</v>
       </c>
     </row>
-    <row r="57" spans="2:10">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13" t="str">
@@ -1920,125 +1923,123 @@
         <v>196.5</v>
       </c>
       <c r="G57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10">
-      <c r="B58" s="45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="41" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="2:10">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="2:10">
-      <c r="B60" s="66" t="s">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="67"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="69"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="64"/>
       <c r="F60" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10">
-      <c r="B61" s="70" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="71"/>
-      <c r="D61" s="71"/>
-      <c r="E61" s="72" t="s">
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="67" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="2:10">
-      <c r="B62" s="70" t="s">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B62" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="72">
+      <c r="C62" s="66"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="67">
         <f>E28</f>
         <v>6550</v>
       </c>
     </row>
-    <row r="63" spans="2:10">
-      <c r="B63" s="70" t="s">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="71"/>
-      <c r="D63" s="71"/>
-      <c r="E63" s="72">
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="67">
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10">
-      <c r="B64" s="73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="74"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="75">
+      <c r="C64" s="69"/>
+      <c r="D64" s="69"/>
+      <c r="E64" s="70">
         <f>SUM(E62*E63)/I6</f>
         <v>3.2749999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
-      <c r="B65" s="76" t="s">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B65" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="71"/>
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="B66" s="33"/>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="B67" s="33"/>
-      <c r="D67" s="34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="37"/>
+      <c r="C65" s="66"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="66"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+      <c r="D67" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B68" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="D68" t="s">
+        <v>48</v>
+      </c>
+      <c r="E68" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D68" t="s">
-        <v>49</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="F68" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G68" s="10"/>
       <c r="H68" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" s="37"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B69" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D69">
         <v>40</v>
       </c>
       <c r="E69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F69" t="str">
         <f>C3</f>
@@ -2049,23 +2050,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="37"/>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70" s="12"/>
       <c r="H70" s="6"/>
     </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="38"/>
-      <c r="B71" s="35"/>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="17"/>
+      <c r="B71" s="34"/>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
-      <c r="H71" s="36"/>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="37"/>
+      <c r="H71" s="35"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B72" s="15"/>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
@@ -2074,20 +2073,9 @@
       <c r="G72" s="13"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="37"/>
-      <c r="H73" s="37"/>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="37"/>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -2098,18 +2086,15 @@
       <c r="I74" s="10"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="37"/>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B75" s="12"/>
       <c r="J75" s="6"/>
     </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="37"/>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B76" s="12"/>
       <c r="J76" s="6"/>
     </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="37"/>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B77" s="15"/>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -2120,46 +2105,36 @@
       <c r="I77" s="13"/>
       <c r="J77" s="9"/>
     </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="37"/>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="37"/>
-    </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" t="s">
         <v>87</v>
       </c>
-      <c r="D79" t="s">
-        <v>88</v>
-      </c>
       <c r="E79" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F79" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C80">
         <f>SUM(E30+E37+E42+D69)</f>
         <v>3977</v>
       </c>
       <c r="D80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E80">
         <f>SUM(C80/I3)</f>
         <v>147.2962962962963</v>
       </c>
-      <c r="F80" s="39">
+      <c r="F80" s="36">
         <v>0.1</v>
       </c>
       <c r="G80">
@@ -2171,22 +2146,22 @@
         <v>162.02592592592595</v>
       </c>
     </row>
-    <row r="81" spans="2:10">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B81" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C81">
         <f>SUM(F56)</f>
         <v>16375</v>
       </c>
       <c r="D81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E81">
         <f>SUM(C81/H4)</f>
         <v>818.75</v>
       </c>
-      <c r="F81" s="39">
+      <c r="F81" s="36">
         <v>0.1</v>
       </c>
       <c r="G81">
@@ -2198,22 +2173,22 @@
         <v>900.625</v>
       </c>
     </row>
-    <row r="82" spans="2:10">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C82">
         <f>SUM(E49)</f>
         <v>4323</v>
       </c>
       <c r="D82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E82">
         <f>SUM(C82/I5)</f>
         <v>160.11111111111111</v>
       </c>
-      <c r="F82" s="39">
+      <c r="F82" s="36">
         <v>0.1</v>
       </c>
       <c r="G82">
@@ -2225,22 +2200,22 @@
         <v>176.12222222222223</v>
       </c>
     </row>
-    <row r="83" spans="2:10">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C83">
         <f>SUM(E62)</f>
         <v>6550</v>
       </c>
       <c r="D83" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E83">
         <f>SUM(C83/I6)</f>
         <v>3.2749999999999999</v>
       </c>
-      <c r="F83" s="39">
+      <c r="F83" s="36">
         <v>0.1</v>
       </c>
       <c r="G83">
@@ -2252,11 +2227,11 @@
         <v>3.6025</v>
       </c>
     </row>
-    <row r="84" spans="2:10">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>59</v>
-      </c>
-      <c r="F84" s="39">
+        <v>58</v>
+      </c>
+      <c r="F84" s="36">
         <v>0.1</v>
       </c>
       <c r="G84">
@@ -2268,22 +2243,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:10">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B85" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C85">
         <f>SUM(F57)</f>
         <v>196.5</v>
       </c>
       <c r="D85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E85" s="19">
         <f>SUM(C85/H8)</f>
         <v>196.5</v>
       </c>
-      <c r="F85" s="39">
+      <c r="F85" s="36">
         <v>0.1</v>
       </c>
       <c r="G85">
@@ -2295,22 +2270,22 @@
         <v>216.15</v>
       </c>
     </row>
-    <row r="86" spans="2:10">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B86" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B87" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10">
-      <c r="B89" s="33"/>
-    </row>
-    <row r="90" spans="2:10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C90" s="10"/>
       <c r="D90" s="10"/>
@@ -2321,15 +2296,15 @@
       <c r="I90" s="10"/>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="2:10">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B91" s="12"/>
       <c r="J91" s="6"/>
     </row>
-    <row r="92" spans="2:10">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B92" s="12"/>
       <c r="J92" s="6"/>
     </row>
-    <row r="93" spans="2:10">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B93" s="15"/>
       <c r="C93" s="13"/>
       <c r="D93" s="13"/>
@@ -2340,15 +2315,15 @@
       <c r="I93" s="13"/>
       <c r="J93" s="9"/>
     </row>
-    <row r="95" spans="2:10">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B95" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C95" s="14"/>
     </row>
-    <row r="96" spans="2:10">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B96" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
@@ -2358,33 +2333,39 @@
         <v>700</v>
       </c>
     </row>
-    <row r="97" spans="2:8">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G97" s="6" t="str">
         <f>C9</f>
         <v>Wood form</v>
       </c>
     </row>
-    <row r="98" spans="2:8">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B98" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G98" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:8">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B99" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G99" s="41">
+        <v>93</v>
+      </c>
+      <c r="G99" s="6">
         <f>SUM(G96)</f>
         <v>700</v>
       </c>
-    </row>
-    <row r="100" spans="2:8">
+      <c r="I99" t="s">
+        <v>121</v>
+      </c>
+      <c r="J99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B100" s="15" t="s">
         <v>13</v>
       </c>
@@ -2396,53 +2377,63 @@
         <f>SUM(G96*G98)/I9</f>
         <v>21.875</v>
       </c>
-    </row>
-    <row r="101" spans="2:8">
+      <c r="I100" s="19">
+        <f>H9</f>
+        <v>16</v>
+      </c>
+      <c r="J100" s="19">
+        <f>I9</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B101" s="12"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="40"/>
-    </row>
-    <row r="102" spans="2:8">
+      <c r="G101" s="37"/>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B102" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G102" s="6">
         <v>700</v>
       </c>
     </row>
-    <row r="103" spans="2:8">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B103" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G103" s="6" t="str">
         <f>C4</f>
         <v>Rebar</v>
       </c>
       <c r="H103" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B104" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G104" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B105" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G105" s="6">
         <f>SUM(G102)</f>
         <v>700</v>
       </c>
-    </row>
-    <row r="106" spans="2:8" ht="14.4" thickBot="1">
+      <c r="I105" t="s">
+        <v>122</v>
+      </c>
+      <c r="J105" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="15" t="s">
         <v>13</v>
       </c>
@@ -2452,51 +2443,58 @@
       <c r="F106" s="13"/>
       <c r="G106" s="9">
         <f>SUM(G102*G104)/H4</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="107" spans="2:8" ht="14.4" thickBot="1">
+        <v>35</v>
+      </c>
+      <c r="I106">
+        <f>H4</f>
+        <v>20</v>
+      </c>
+      <c r="J106" s="19">
+        <f>I4</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="2:8">
-      <c r="B108" s="37"/>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D108" t="s">
+        <v>95</v>
+      </c>
+      <c r="E108" t="s">
+        <v>25</v>
+      </c>
+      <c r="F108" t="s">
+        <v>91</v>
+      </c>
+      <c r="G108" t="s">
         <v>96</v>
       </c>
-      <c r="E108" t="s">
-        <v>26</v>
-      </c>
-      <c r="F108" t="s">
-        <v>92</v>
-      </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>97</v>
       </c>
-      <c r="H108" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8">
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B109" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C109">
         <f>SUM(G102)</f>
         <v>700</v>
       </c>
       <c r="D109" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E109" s="20">
         <f>SUM(C109/H9)</f>
         <v>43.75</v>
       </c>
-      <c r="F109" s="39">
+      <c r="F109" s="36">
         <v>0.1</v>
       </c>
       <c r="G109">
@@ -2508,22 +2506,22 @@
         <v>48.125</v>
       </c>
     </row>
-    <row r="110" spans="2:8">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B110" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C110">
         <f>SUM(G105)</f>
         <v>700</v>
       </c>
       <c r="D110" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E110" s="20">
         <f>SUM(C110/H10)</f>
         <v>43.75</v>
       </c>
-      <c r="F110" s="39">
+      <c r="F110" s="36">
         <v>0.1</v>
       </c>
       <c r="G110">
@@ -2535,21 +2533,17 @@
         <v>48.125</v>
       </c>
     </row>
-    <row r="111" spans="2:8">
-      <c r="B111" s="37"/>
-    </row>
-    <row r="114" spans="2:6">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C114" s="37"/>
+        <v>72</v>
+      </c>
       <c r="D114" s="10"/>
       <c r="E114" s="10"/>
       <c r="F114" s="4"/>
     </row>
-    <row r="115" spans="2:6">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D115" t="str">
         <f>C11</f>
@@ -2560,17 +2554,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:6">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B116" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F116" s="30">
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="2:6">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B117" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C117" s="13"/>
       <c r="D117" s="13"/>

</xml_diff>